<commit_message>
Sprint 2 release backlog
</commit_message>
<xml_diff>
--- a/Documents/Tasks Planning.xlsx
+++ b/Documents/Tasks Planning.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\EMSI\4IIR\S2\PFA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\EMSI\4IIR\S2\PFA\i-Mark\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4454D1-D784-48D1-95B9-B5CF81D9EC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6EA9F9-1BBD-4B20-959B-04367E70F516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{2B6B036F-760A-4B36-95D1-DDEE59172969}"/>
   </bookViews>
@@ -98,12 +98,6 @@
     <t>Etude benchmark</t>
   </si>
   <si>
-    <t>Planning prévisionnel (Mise ajour)</t>
-  </si>
-  <si>
-    <t>Charte du projet (Mise ajour)</t>
-  </si>
-  <si>
     <t>Réalisation des premières fonctionnalités</t>
   </si>
   <si>
@@ -131,10 +125,16 @@
     <t>30/4/2022</t>
   </si>
   <si>
-    <t>20/4/2022</t>
-  </si>
-  <si>
     <t>11 Avril - 29 Avril</t>
+  </si>
+  <si>
+    <t>Charte du projet (Mise a jour)</t>
+  </si>
+  <si>
+    <t>Planning prévisionnel (Mise a jour)</t>
+  </si>
+  <si>
+    <t>20/5/2022</t>
   </si>
 </sst>
 </file>
@@ -513,26 +513,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -582,6 +564,54 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -591,43 +621,13 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -946,347 +946,347 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404DFDD5-7BB4-4413-8FC5-303AC07517DF}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.7265625" style="43" customWidth="1"/>
-    <col min="2" max="2" width="36.6328125" style="43" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" style="43" customWidth="1"/>
-    <col min="4" max="5" width="25.6328125" style="43" customWidth="1"/>
+    <col min="1" max="1" width="36.7265625" style="34" customWidth="1"/>
+    <col min="2" max="2" width="36.6328125" style="34" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" style="34" customWidth="1"/>
+    <col min="4" max="5" width="25.6328125" style="34" customWidth="1"/>
     <col min="6" max="16384" width="10.90625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="4" customFormat="1" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="43"/>
+    </row>
+    <row r="4" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>44838</v>
+      </c>
+      <c r="E4" s="7">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1</v>
+      </c>
+      <c r="D5" s="11">
+        <v>44838</v>
+      </c>
+      <c r="E5" s="11">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1</v>
+      </c>
+      <c r="D6" s="13">
+        <v>44838</v>
+      </c>
+      <c r="E6" s="14">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10">
+        <v>1</v>
+      </c>
+      <c r="D7" s="16">
+        <v>44838</v>
+      </c>
+      <c r="E7" s="17">
+        <v>44838</v>
+      </c>
+      <c r="F7" s="18"/>
+    </row>
+    <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="21">
+        <v>1</v>
+      </c>
+      <c r="D8" s="14">
+        <v>44838</v>
+      </c>
+      <c r="E8" s="14">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="37"/>
+    </row>
+    <row r="10" spans="1:6" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="40"/>
+    </row>
+    <row r="11" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="22">
+        <v>2</v>
+      </c>
+      <c r="D11" s="23">
+        <v>44869</v>
+      </c>
+      <c r="E11" s="23">
+        <v>44899</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="24">
+        <v>2</v>
+      </c>
+      <c r="D12" s="16">
+        <v>44869</v>
+      </c>
+      <c r="E12" s="25">
+        <v>44899</v>
+      </c>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="10">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16">
+        <v>44869</v>
+      </c>
+      <c r="E13" s="26">
+        <v>44869</v>
+      </c>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="24">
+        <v>1</v>
+      </c>
+      <c r="D14" s="27">
+        <v>44869</v>
+      </c>
+      <c r="E14" s="16">
+        <v>44869</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="12">
+        <v>18</v>
+      </c>
+      <c r="D15" s="13">
+        <v>44899</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="37"/>
+    </row>
+    <row r="17" spans="1:5" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="40"/>
+    </row>
+    <row r="18" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="6">
+        <v>5</v>
+      </c>
+      <c r="D18" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="7" customFormat="1" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:6" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="12">
+      <c r="E18" s="23">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="13">
-        <v>44838</v>
-      </c>
-      <c r="E4" s="13">
-        <v>44838</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="16">
-        <v>1</v>
-      </c>
-      <c r="D5" s="17">
-        <v>44838</v>
-      </c>
-      <c r="E5" s="17">
-        <v>44838</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="14" t="s">
+      <c r="B19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="10">
         <v>2</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="18">
-        <v>1</v>
-      </c>
-      <c r="D6" s="19">
-        <v>44838</v>
-      </c>
-      <c r="E6" s="20">
-        <v>44838</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="14" t="s">
+      <c r="D19" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="16">
+        <v>44566</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="10">
+        <v>21</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="16">
-        <v>1</v>
-      </c>
-      <c r="D7" s="22">
-        <v>44838</v>
-      </c>
-      <c r="E7" s="23">
-        <v>44838</v>
-      </c>
-      <c r="F7" s="24"/>
-    </row>
-    <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="25" t="s">
+      <c r="B21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="24">
+        <v>21</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="27">
-        <v>1</v>
-      </c>
-      <c r="D8" s="20">
-        <v>44838</v>
-      </c>
-      <c r="E8" s="20">
-        <v>44838</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="3" t="s">
+      <c r="B22" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="31">
+        <v>21</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="33" t="s">
         <v>33</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30"/>
-    </row>
-    <row r="11" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="31">
-        <v>2</v>
-      </c>
-      <c r="D11" s="32">
-        <v>44869</v>
-      </c>
-      <c r="E11" s="32">
-        <v>44899</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="33">
-        <v>2</v>
-      </c>
-      <c r="D12" s="22">
-        <v>44869</v>
-      </c>
-      <c r="E12" s="34">
-        <v>44899</v>
-      </c>
-      <c r="F12" s="24"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="16">
-        <v>1</v>
-      </c>
-      <c r="D13" s="22">
-        <v>44869</v>
-      </c>
-      <c r="E13" s="35">
-        <v>44869</v>
-      </c>
-      <c r="F13" s="24"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="33">
-        <v>1</v>
-      </c>
-      <c r="D14" s="36">
-        <v>44869</v>
-      </c>
-      <c r="E14" s="22">
-        <v>44869</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="18">
-        <v>18</v>
-      </c>
-      <c r="D15" s="19">
-        <v>44899</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="30"/>
-    </row>
-    <row r="18" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="12">
-        <v>5</v>
-      </c>
-      <c r="D18" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="32">
-        <v>44656</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="16">
-        <v>2</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="22">
-        <v>44566</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="16">
-        <v>21</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A21" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="33">
-        <v>21</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="40">
-        <v>21</v>
-      </c>
-      <c r="D22" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="42" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.45"/>

</xml_diff>